<commit_message>
added Address table and endpoint
</commit_message>
<xml_diff>
--- a/Documents/DatabaseSchema.xlsx
+++ b/Documents/DatabaseSchema.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\Documents\RKW Website\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\michael.mountford\OneDrive\Programming\matt-mikes-practice\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Item" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">data!$A$1:$G$46</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">data!$A$1:$G$77</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1950" uniqueCount="662">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1953" uniqueCount="663">
   <si>
     <t>Table</t>
   </si>
@@ -2015,6 +2015,9 @@
   </si>
   <si>
     <t>cartonWidth</t>
+  </si>
+  <si>
+    <t>city</t>
   </si>
 </sst>
 </file>
@@ -2342,11 +2345,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H77"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:H78"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F12" sqref="F12"/>
+      <selection pane="bottomLeft" activeCell="A78" sqref="A78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2382,7 +2386,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -2398,7 +2402,7 @@
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -2420,7 +2424,7 @@
       </c>
       <c r="H3" s="1"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -2442,7 +2446,7 @@
       </c>
       <c r="H4" s="1"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -2464,7 +2468,7 @@
       </c>
       <c r="H5" s="1"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -2486,7 +2490,7 @@
       </c>
       <c r="H6" s="1"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>3</v>
       </c>
@@ -2506,7 +2510,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>3</v>
       </c>
@@ -2522,7 +2526,7 @@
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>3</v>
       </c>
@@ -2542,7 +2546,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>3</v>
       </c>
@@ -2562,7 +2566,7 @@
       </c>
       <c r="H10" s="1"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>3</v>
       </c>
@@ -2582,7 +2586,7 @@
       </c>
       <c r="H11" s="1"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>3</v>
       </c>
@@ -2602,7 +2606,7 @@
       </c>
       <c r="H12" s="1"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>3</v>
       </c>
@@ -2622,7 +2626,7 @@
       </c>
       <c r="H13" s="1"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>3</v>
       </c>
@@ -2644,7 +2648,7 @@
       </c>
       <c r="H14" s="1"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>3</v>
       </c>
@@ -2666,7 +2670,7 @@
       </c>
       <c r="H15" s="1"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>3</v>
       </c>
@@ -2688,7 +2692,7 @@
       </c>
       <c r="H16" s="1"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>3</v>
       </c>
@@ -2710,7 +2714,7 @@
       </c>
       <c r="H17" s="1"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>3</v>
       </c>
@@ -2732,7 +2736,7 @@
       </c>
       <c r="H18" s="1"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>3</v>
       </c>
@@ -2754,7 +2758,7 @@
       </c>
       <c r="H19" s="1"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>3</v>
       </c>
@@ -2776,7 +2780,7 @@
       </c>
       <c r="H20" s="1"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>3</v>
       </c>
@@ -2798,7 +2802,7 @@
       </c>
       <c r="H21" s="1"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>3</v>
       </c>
@@ -2820,7 +2824,7 @@
       </c>
       <c r="H22" s="1"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>3</v>
       </c>
@@ -2840,7 +2844,7 @@
       </c>
       <c r="H23" s="1"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>3</v>
       </c>
@@ -2860,7 +2864,7 @@
       </c>
       <c r="H24" s="1"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>3</v>
       </c>
@@ -2880,7 +2884,7 @@
       </c>
       <c r="H25" s="1"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>3</v>
       </c>
@@ -2900,7 +2904,7 @@
       </c>
       <c r="H26" s="1"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>3</v>
       </c>
@@ -2920,7 +2924,7 @@
       </c>
       <c r="H27" s="1"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>3</v>
       </c>
@@ -2940,7 +2944,7 @@
       </c>
       <c r="H28" s="1"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>3</v>
       </c>
@@ -2960,7 +2964,7 @@
       </c>
       <c r="H29" s="1"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>3</v>
       </c>
@@ -2980,7 +2984,7 @@
       </c>
       <c r="H30" s="1"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>3</v>
       </c>
@@ -3000,7 +3004,7 @@
       </c>
       <c r="H31" s="1"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>3</v>
       </c>
@@ -3020,7 +3024,7 @@
       </c>
       <c r="H32" s="1"/>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>3</v>
       </c>
@@ -3040,7 +3044,7 @@
       </c>
       <c r="H33" s="1"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>3</v>
       </c>
@@ -3060,7 +3064,7 @@
       </c>
       <c r="H34" s="1"/>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>3</v>
       </c>
@@ -3080,7 +3084,7 @@
       </c>
       <c r="H35" s="1"/>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>3</v>
       </c>
@@ -3100,7 +3104,7 @@
       </c>
       <c r="H36" s="1"/>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>626</v>
       </c>
@@ -3116,7 +3120,7 @@
       <c r="G37" s="1"/>
       <c r="H37" s="1"/>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>626</v>
       </c>
@@ -3132,7 +3136,7 @@
       <c r="G38" s="1"/>
       <c r="H38" s="1"/>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>626</v>
       </c>
@@ -3148,7 +3152,7 @@
       <c r="G39" s="1"/>
       <c r="H39" s="1"/>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>626</v>
       </c>
@@ -3164,7 +3168,7 @@
       <c r="G40" s="1"/>
       <c r="H40" s="1"/>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>626</v>
       </c>
@@ -3180,7 +3184,7 @@
       <c r="G41" s="1"/>
       <c r="H41" s="1"/>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>632</v>
       </c>
@@ -3191,7 +3195,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>632</v>
       </c>
@@ -3202,7 +3206,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>632</v>
       </c>
@@ -3213,7 +3217,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>632</v>
       </c>
@@ -3224,7 +3228,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>632</v>
       </c>
@@ -3364,7 +3368,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>645</v>
       </c>
@@ -3375,7 +3379,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>645</v>
       </c>
@@ -3386,7 +3390,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>645</v>
       </c>
@@ -3397,7 +3401,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>645</v>
       </c>
@@ -3408,7 +3412,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>645</v>
       </c>
@@ -3419,7 +3423,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>613</v>
       </c>
@@ -3430,7 +3434,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>613</v>
       </c>
@@ -3441,7 +3445,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>613</v>
       </c>
@@ -3452,7 +3456,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>613</v>
       </c>
@@ -3463,7 +3467,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>613</v>
       </c>
@@ -3474,7 +3478,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>613</v>
       </c>
@@ -3485,7 +3489,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>652</v>
       </c>
@@ -3494,7 +3498,7 @@
       </c>
       <c r="C68" s="1"/>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>652</v>
       </c>
@@ -3505,7 +3509,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>652</v>
       </c>
@@ -3516,7 +3520,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>652</v>
       </c>
@@ -3527,7 +3531,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>652</v>
       </c>
@@ -3538,7 +3542,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>652</v>
       </c>
@@ -3549,7 +3553,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>652</v>
       </c>
@@ -3560,7 +3564,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>657</v>
       </c>
@@ -3568,7 +3572,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>657</v>
       </c>
@@ -3576,7 +3580,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>657</v>
       </c>
@@ -3584,8 +3588,28 @@
         <v>658</v>
       </c>
     </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78" s="1" t="s">
+        <v>634</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>662</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>623</v>
+      </c>
+      <c r="D78">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:G46"/>
+  <autoFilter ref="A1:G77">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="Address"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>